<commit_message>
datasync, #215: Review of datasync test.
</commit_message>
<xml_diff>
--- a/tests/datasync.xlsx
+++ b/tests/datasync.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/input/datasync/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17025" yWindow="-15" windowWidth="17040" windowHeight="15225" activeTab="2"/>
+    <workbookView xWindow="11760" yWindow="460" windowWidth="17040" windowHeight="15220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,17 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
   <si>
     <t>x</t>
   </si>
@@ -29,9 +39,6 @@
   </si>
   <si>
     <t>y3</t>
-  </si>
-  <si>
-    <t>Y_RESAMPLE</t>
   </si>
 </sst>
 </file>
@@ -126,7 +133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -161,7 +168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -372,13 +379,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -400,7 +407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -411,7 +418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -422,7 +429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -433,7 +440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -444,276 +451,276 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C25">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>58</v>
@@ -728,11 +735,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,9 +755,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -760,9 +769,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -774,9 +783,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -788,9 +797,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -802,9 +811,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -816,12 +825,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -830,12 +839,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -844,12 +853,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -858,12 +867,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -872,12 +881,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>18</v>
@@ -886,12 +895,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -900,12 +909,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>22</v>
@@ -914,12 +923,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>24</v>
@@ -928,12 +937,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>26</v>
@@ -942,12 +951,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>28</v>
@@ -956,12 +965,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>30</v>
@@ -970,12 +979,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>32</v>
@@ -984,12 +993,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>34</v>
@@ -998,12 +1007,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>36</v>
@@ -1012,12 +1021,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>38</v>
@@ -1026,12 +1035,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>40</v>
@@ -1040,12 +1049,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>42</v>
@@ -1054,12 +1063,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>44</v>
@@ -1068,12 +1077,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C25">
         <v>46</v>
@@ -1082,12 +1091,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B26">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>48</v>
@@ -1096,12 +1105,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B27">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>50</v>
@@ -1110,12 +1119,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B28">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>52</v>
@@ -1124,12 +1133,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>54</v>
@@ -1138,12 +1147,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>56</v>
@@ -1152,12 +1161,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>58</v>
@@ -1173,15 +1182,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1189,12 +1198,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1202,643 +1214,344 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1.5</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3.5</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>4.5</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>5.5</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>6.5</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>6.5</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>7.5</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>7.5</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>8.5</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="D20">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>9.5</v>
+        <v>27</v>
       </c>
       <c r="B21">
-        <v>9.5</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="D21">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10.5</v>
+        <v>29</v>
       </c>
       <c r="B23">
-        <v>10.5</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="D24">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>11.5</v>
+        <v>32</v>
       </c>
       <c r="B25">
-        <v>11.5</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>12.5</v>
-      </c>
-      <c r="B27">
-        <v>12.5</v>
-      </c>
-      <c r="C27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>13</v>
-      </c>
-      <c r="B28">
-        <v>13</v>
-      </c>
-      <c r="C28">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>13.5</v>
-      </c>
-      <c r="B29">
-        <v>13.5</v>
-      </c>
-      <c r="C29">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>14</v>
-      </c>
-      <c r="B30">
-        <v>14</v>
-      </c>
-      <c r="C30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>14.5</v>
-      </c>
-      <c r="B31">
-        <v>14.5</v>
-      </c>
-      <c r="C31">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>15</v>
-      </c>
-      <c r="B32">
-        <v>15</v>
-      </c>
-      <c r="C32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>15.5</v>
-      </c>
-      <c r="B33">
-        <v>15.5</v>
-      </c>
-      <c r="C33">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>16</v>
-      </c>
-      <c r="B34">
-        <v>16</v>
-      </c>
-      <c r="C34">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>16.5</v>
-      </c>
-      <c r="B35">
-        <v>16.5</v>
-      </c>
-      <c r="C35">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>17</v>
-      </c>
-      <c r="B36">
-        <v>17</v>
-      </c>
-      <c r="C36">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>17.5</v>
-      </c>
-      <c r="B37">
-        <v>17.5</v>
-      </c>
-      <c r="C37">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>18</v>
-      </c>
-      <c r="B38">
-        <v>18</v>
-      </c>
-      <c r="C38">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>18.5</v>
-      </c>
-      <c r="B39">
-        <v>18.5</v>
-      </c>
-      <c r="C39">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>19</v>
-      </c>
-      <c r="B40">
-        <v>19</v>
-      </c>
-      <c r="C40">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>19.5</v>
-      </c>
-      <c r="B41">
-        <v>19.5</v>
-      </c>
-      <c r="C41">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>20</v>
-      </c>
-      <c r="B42">
-        <v>20</v>
-      </c>
-      <c r="C42">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>20.5</v>
-      </c>
-      <c r="B43">
-        <v>20.5</v>
-      </c>
-      <c r="C43">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>21</v>
-      </c>
-      <c r="B44">
-        <v>21</v>
-      </c>
-      <c r="C44">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>21.5</v>
-      </c>
-      <c r="B45">
-        <v>21.5</v>
-      </c>
-      <c r="C45">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>22</v>
-      </c>
-      <c r="B46">
-        <v>22</v>
-      </c>
-      <c r="C46">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>22.5</v>
-      </c>
-      <c r="B47">
-        <v>22.5</v>
-      </c>
-      <c r="C47">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>23</v>
-      </c>
-      <c r="B48">
-        <v>23</v>
-      </c>
-      <c r="C48">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>23.5</v>
-      </c>
-      <c r="B49">
-        <v>23.5</v>
-      </c>
-      <c r="C49">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>24</v>
-      </c>
-      <c r="B50">
-        <v>24</v>
-      </c>
-      <c r="C50">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>24.5</v>
-      </c>
-      <c r="B51">
-        <v>24.5</v>
-      </c>
-      <c r="C51">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>25</v>
-      </c>
-      <c r="B52">
-        <v>25</v>
-      </c>
-      <c r="C52">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>25.5</v>
-      </c>
-      <c r="B53">
-        <v>25.5</v>
-      </c>
-      <c r="C53">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>26</v>
-      </c>
-      <c r="B54">
-        <v>26</v>
-      </c>
-      <c r="C54">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>26.5</v>
-      </c>
-      <c r="B55">
-        <v>26.5</v>
-      </c>
-      <c r="C55">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>27</v>
-      </c>
-      <c r="B56">
-        <v>27</v>
-      </c>
-      <c r="C56">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>27.5</v>
-      </c>
-      <c r="B57">
-        <v>27.5</v>
-      </c>
-      <c r="C57">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>28</v>
-      </c>
-      <c r="B58">
-        <v>28</v>
-      </c>
-      <c r="C58">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>28.5</v>
-      </c>
-      <c r="B59">
-        <v>28.5</v>
-      </c>
-      <c r="C59">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>29</v>
-      </c>
-      <c r="B60">
-        <v>29</v>
-      </c>
-      <c r="C60">
         <v>58</v>
+      </c>
+      <c r="D26">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1565,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#144,datasync: Test also resamplings.
+ Add 1 more sheets to be synced.
- NOW 8 more TCs FAIL due to UNSTABLE of sheet-ordering.
- Still 5 TCas fail due to urls.
</commit_message>
<xml_diff>
--- a/tests/datasync.xlsx
+++ b/tests/datasync.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="17025" yWindow="-15" windowWidth="17040" windowHeight="15225"/>
+    <workbookView xWindow="17025" yWindow="-15" windowWidth="17040" windowHeight="15225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>x</t>
   </si>
@@ -28,6 +29,9 @@
   </si>
   <si>
     <t>y3</t>
+  </si>
+  <si>
+    <t>Y_RESAMPLE</t>
   </si>
 </sst>
 </file>
@@ -368,7 +372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1167,6 +1173,681 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.5</v>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2.5</v>
+      </c>
+      <c r="B7">
+        <v>2.5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3.5</v>
+      </c>
+      <c r="B9">
+        <v>3.5</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.5</v>
+      </c>
+      <c r="B11">
+        <v>4.5</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5.5</v>
+      </c>
+      <c r="B13">
+        <v>5.5</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6.5</v>
+      </c>
+      <c r="B15">
+        <v>6.5</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7.5</v>
+      </c>
+      <c r="B17">
+        <v>7.5</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8.5</v>
+      </c>
+      <c r="B19">
+        <v>8.5</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>9.5</v>
+      </c>
+      <c r="B21">
+        <v>9.5</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10.5</v>
+      </c>
+      <c r="B23">
+        <v>10.5</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>11.5</v>
+      </c>
+      <c r="B25">
+        <v>11.5</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12.5</v>
+      </c>
+      <c r="B27">
+        <v>12.5</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>13.5</v>
+      </c>
+      <c r="B29">
+        <v>13.5</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>14.5</v>
+      </c>
+      <c r="B31">
+        <v>14.5</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>15.5</v>
+      </c>
+      <c r="B33">
+        <v>15.5</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>16</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>16.5</v>
+      </c>
+      <c r="B35">
+        <v>16.5</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>17.5</v>
+      </c>
+      <c r="B37">
+        <v>17.5</v>
+      </c>
+      <c r="C37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>18</v>
+      </c>
+      <c r="B38">
+        <v>18</v>
+      </c>
+      <c r="C38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>18.5</v>
+      </c>
+      <c r="B39">
+        <v>18.5</v>
+      </c>
+      <c r="C39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>19</v>
+      </c>
+      <c r="B40">
+        <v>19</v>
+      </c>
+      <c r="C40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>19.5</v>
+      </c>
+      <c r="B41">
+        <v>19.5</v>
+      </c>
+      <c r="C41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>20</v>
+      </c>
+      <c r="C42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>20.5</v>
+      </c>
+      <c r="B43">
+        <v>20.5</v>
+      </c>
+      <c r="C43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>21</v>
+      </c>
+      <c r="B44">
+        <v>21</v>
+      </c>
+      <c r="C44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>21.5</v>
+      </c>
+      <c r="B45">
+        <v>21.5</v>
+      </c>
+      <c r="C45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>22</v>
+      </c>
+      <c r="B46">
+        <v>22</v>
+      </c>
+      <c r="C46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>22.5</v>
+      </c>
+      <c r="B47">
+        <v>22.5</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>23</v>
+      </c>
+      <c r="B48">
+        <v>23</v>
+      </c>
+      <c r="C48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>23.5</v>
+      </c>
+      <c r="B49">
+        <v>23.5</v>
+      </c>
+      <c r="C49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>24</v>
+      </c>
+      <c r="B50">
+        <v>24</v>
+      </c>
+      <c r="C50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>24.5</v>
+      </c>
+      <c r="B51">
+        <v>24.5</v>
+      </c>
+      <c r="C51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>25</v>
+      </c>
+      <c r="B52">
+        <v>25</v>
+      </c>
+      <c r="C52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>25.5</v>
+      </c>
+      <c r="B53">
+        <v>25.5</v>
+      </c>
+      <c r="C53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>26</v>
+      </c>
+      <c r="B54">
+        <v>26</v>
+      </c>
+      <c r="C54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>26.5</v>
+      </c>
+      <c r="B55">
+        <v>26.5</v>
+      </c>
+      <c r="C55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>27</v>
+      </c>
+      <c r="B56">
+        <v>27</v>
+      </c>
+      <c r="C56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>27.5</v>
+      </c>
+      <c r="B57">
+        <v>27.5</v>
+      </c>
+      <c r="C57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>28</v>
+      </c>
+      <c r="B58">
+        <v>28</v>
+      </c>
+      <c r="C58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>28.5</v>
+      </c>
+      <c r="B59">
+        <v>28.5</v>
+      </c>
+      <c r="C59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>29</v>
+      </c>
+      <c r="B60">
+        <v>29</v>
+      </c>
+      <c r="C60">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
datasync(#218): AMIDST make datasync a separate cmd-line entry-point.
+ datasync:
  + Properly use xleash to simplify cmd-line args.
  + FIX  absolute but NOT url-files.
  + Cmd now runs a a single sync (not in a loop).
+ main: remove datasync.
+ TCs:
  + Replace csv with inline-text.
  + FIX expected df column-parsing not to introduce suffixes.
docs: Add datasync section.
</commit_message>
<xml_diff>
--- a/tests/datasync.xlsx
+++ b/tests/datasync.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/input/datasync/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="460" windowWidth="17040" windowHeight="15220"/>
+    <workbookView xWindow="11760" yWindow="465" windowWidth="17040" windowHeight="15225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>x</t>
   </si>
@@ -39,6 +34,9 @@
   </si>
   <si>
     <t>y3</t>
+  </si>
+  <si>
+    <t>OtherY</t>
   </si>
 </sst>
 </file>
@@ -133,7 +131,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,7 +166,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,11 +377,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -735,11 +731,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1184,11 +1178,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1201,7 +1193,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1565,7 +1557,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>